<commit_message>
aggiunto file .bat per aggiornamento file .csv, .c e .h. Aggiornato database
</commit_message>
<xml_diff>
--- a/db/ike_params_process_data.xlsx
+++ b/db/ike_params_process_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\local_repos\_private\ike_gui\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1E13B3-3AC1-48E2-9B4A-52A5641718D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B132CA49-E849-4814-8B31-1206A0242541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{35ECC9C5-EA02-4EE7-AAE2-09095EF705F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{35ECC9C5-EA02-4EE7-AAE2-09095EF705F3}"/>
   </bookViews>
   <sheets>
     <sheet name="params_data" sheetId="9" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="142">
   <si>
     <t>type</t>
   </si>
@@ -89,24 +89,6 @@
     <t>adc.adc_ctrl_fdb_rect.i_inv_rect_offset</t>
   </si>
   <si>
-    <t>adc.adc_sys.ntc1_gain</t>
-  </si>
-  <si>
-    <t>adc.adc_sys.ntc1_offset</t>
-  </si>
-  <si>
-    <t>adc.adc_sys.ntc2_gain</t>
-  </si>
-  <si>
-    <t>adc.adc_sys.ntc2_offset</t>
-  </si>
-  <si>
-    <t>adc.adc_sys.pot_gain</t>
-  </si>
-  <si>
-    <t>adc.adc_sys.pot_offset</t>
-  </si>
-  <si>
     <t>PROTECTION</t>
   </si>
   <si>
@@ -194,24 +176,6 @@
     <t>adattamento adc i_inv_rect_offset</t>
   </si>
   <si>
-    <t>adattamento adc ntc1_gain</t>
-  </si>
-  <si>
-    <t>adattamento adc ntc1_offset</t>
-  </si>
-  <si>
-    <t>adattamento adc ntc2_gain</t>
-  </si>
-  <si>
-    <t>adattamento adc ntc2_offset</t>
-  </si>
-  <si>
-    <t>adattamento adc pot_gain</t>
-  </si>
-  <si>
-    <t>adattamento adc pot_offset</t>
-  </si>
-  <si>
     <t>valore di scatto sovracorrente AC</t>
   </si>
   <si>
@@ -428,9 +392,6 @@
     <t>diagn_out.db_version</t>
   </si>
   <si>
-    <t>02.03.01</t>
-  </si>
-  <si>
     <t>perc</t>
   </si>
   <si>
@@ -491,7 +452,22 @@
     <t>igbt_out.igbt_actual_freq</t>
   </si>
   <si>
-    <t>10ms</t>
+    <t>V/u16</t>
+  </si>
+  <si>
+    <t>A/u16</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>scr_sett.scr_cmd_alfa_max</t>
+  </si>
+  <si>
+    <t>valore massimo apertura scr</t>
+  </si>
+  <si>
+    <t>01.02.03</t>
   </si>
 </sst>
 </file>
@@ -911,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041AAE19-AD56-4293-9964-80E5B30A6810}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +902,7 @@
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1"/>
@@ -938,7 +914,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -947,13 +923,13 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -965,7 +941,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>5</v>
@@ -974,16 +950,16 @@
         <v>1</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -994,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -1016,41 +992,41 @@
         <v>65535</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="M2" s="7">
-        <f t="shared" ref="M2:M26" si="0">65535/(I2-H2)</f>
+        <f t="shared" ref="M2:M21" si="0">65535/(I2-H2)</f>
         <v>1</v>
       </c>
       <c r="N2" s="7">
-        <f t="shared" ref="N2:N26" si="1">1/M2</f>
+        <f t="shared" ref="N2:N21" si="1">1/M2</f>
         <v>1</v>
       </c>
       <c r="O2" s="7">
-        <f t="shared" ref="O2:O26" si="2">1/M2</f>
+        <f t="shared" ref="O2:O21" si="2">1/M2</f>
         <v>1</v>
       </c>
       <c r="P2" s="12">
-        <f t="shared" ref="P2:P26" si="3">ROUND((F2-H2)*M2,0)</f>
+        <f t="shared" ref="P2:P21" si="3">ROUND((F2-H2)*M2,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A26" si="4">A2+1</f>
+        <f t="shared" ref="A3:A21" si="4">A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1059,38 +1035,38 @@
         <v>10</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F26" si="5">G3</f>
-        <v>100</v>
+        <f t="shared" ref="F3:F21" si="5">G3</f>
+        <v>1000</v>
       </c>
       <c r="G3" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <v>6553</v>
+        <v>65535</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="0"/>
-        <v>10.000763009308713</v>
+        <v>1</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" si="1"/>
-        <v>9.9992370489051657E-2</v>
+        <v>1</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" si="2"/>
-        <v>9.9992370489051657E-2</v>
+        <v>1</v>
       </c>
       <c r="P3" s="12">
         <f t="shared" si="3"/>
@@ -1106,7 +1082,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -1116,41 +1092,41 @@
       </c>
       <c r="F4" s="2">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="G4" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H4" s="2">
         <v>10</v>
       </c>
       <c r="I4" s="2">
-        <v>1500</v>
+        <v>15000</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="M4" s="7">
         <f t="shared" si="0"/>
-        <v>43.983221476510067</v>
+        <v>4.3719146097398269</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" si="1"/>
-        <v>2.2735942626077667E-2</v>
+        <v>0.22873273823147935</v>
       </c>
       <c r="O4" s="7">
         <f t="shared" si="2"/>
-        <v>2.2735942626077667E-2</v>
+        <v>0.22873273823147935</v>
       </c>
       <c r="P4" s="12">
         <f t="shared" si="3"/>
-        <v>3958</v>
+        <v>4328</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -1162,7 +1138,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -1184,13 +1160,13 @@
         <v>65535</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="0"/>
@@ -1218,7 +1194,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
@@ -1240,13 +1216,13 @@
         <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="M6" s="7">
         <f t="shared" si="0"/>
@@ -1274,51 +1250,51 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="3">
-        <f t="shared" si="5"/>
-        <v>0.05</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>1</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>38</v>
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F7" s="4">
+        <f>G7</f>
+        <v>0.95</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="M7" s="7">
-        <f t="shared" si="0"/>
-        <v>65535</v>
+        <f>65535/(I7-H7)</f>
+        <v>93621.42857142858</v>
       </c>
       <c r="N7" s="7">
-        <f t="shared" si="1"/>
-        <v>1.5259021896696422E-5</v>
+        <f>1/M7</f>
+        <v>1.0681315327687494E-5</v>
       </c>
       <c r="O7" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5259021896696422E-5</v>
+        <f>1/M7</f>
+        <v>1.0681315327687494E-5</v>
       </c>
       <c r="P7" s="12">
-        <f t="shared" si="3"/>
-        <v>3277</v>
+        <f>ROUND((F7-H7)*M7,0)</f>
+        <v>60854</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -1330,7 +1306,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
@@ -1339,7 +1315,7 @@
         <v>0.1</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="5"/>
+        <f>G8</f>
         <v>0.05</v>
       </c>
       <c r="G8" s="3">
@@ -1352,28 +1328,28 @@
         <v>1</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="M8" s="7">
-        <f t="shared" si="0"/>
+        <f>65535/(I8-H8)</f>
         <v>65535</v>
       </c>
       <c r="N8" s="7">
-        <f t="shared" si="1"/>
+        <f>1/M8</f>
         <v>1.5259021896696422E-5</v>
       </c>
       <c r="O8" s="7">
-        <f t="shared" si="2"/>
+        <f>1/M8</f>
         <v>1.5259021896696422E-5</v>
       </c>
       <c r="P8" s="12">
-        <f t="shared" si="3"/>
+        <f>ROUND((F8-H8)*M8,0)</f>
         <v>3277</v>
       </c>
     </row>
@@ -1386,51 +1362,51 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="5"/>
-        <v>200</v>
-      </c>
-      <c r="G9" s="2">
-        <v>200</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
-        <v>6553</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>149</v>
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="3">
+        <f>G9</f>
+        <v>0.05</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="M9" s="7">
-        <f t="shared" si="0"/>
-        <v>10.000763009308713</v>
+        <f>65535/(I9-H9)</f>
+        <v>65535</v>
       </c>
       <c r="N9" s="7">
-        <f t="shared" si="1"/>
-        <v>9.9992370489051657E-2</v>
+        <f>1/M9</f>
+        <v>1.5259021896696422E-5</v>
       </c>
       <c r="O9" s="7">
-        <f t="shared" si="2"/>
-        <v>9.9992370489051657E-2</v>
+        <f>1/M9</f>
+        <v>1.5259021896696422E-5</v>
       </c>
       <c r="P9" s="12">
-        <f t="shared" si="3"/>
-        <v>2000</v>
+        <f>ROUND((F9-H9)*M9,0)</f>
+        <v>3277</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -1442,7 +1418,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -1451,42 +1427,42 @@
         <v>10</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="5"/>
-        <v>600</v>
+        <f>G10</f>
+        <v>2000</v>
       </c>
       <c r="G10" s="2">
-        <v>600</v>
+        <v>2000</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
       </c>
       <c r="I10" s="2">
-        <v>6553</v>
+        <v>65535</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="M10" s="7">
-        <f t="shared" si="0"/>
-        <v>10.000763009308713</v>
+        <f>65535/(I10-H10)</f>
+        <v>1</v>
       </c>
       <c r="N10" s="7">
-        <f t="shared" si="1"/>
-        <v>9.9992370489051657E-2</v>
+        <f>1/M10</f>
+        <v>1</v>
       </c>
       <c r="O10" s="7">
-        <f t="shared" si="2"/>
-        <v>9.9992370489051657E-2</v>
+        <f>1/M10</f>
+        <v>1</v>
       </c>
       <c r="P10" s="12">
-        <f t="shared" si="3"/>
-        <v>6000</v>
+        <f>ROUND((F10-H10)*M10,0)</f>
+        <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -1495,54 +1471,54 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
+        <v>6000</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6000</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
         <v>65535</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>29</v>
+      <c r="J11" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>142</v>
+        <v>36</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="M11" s="7">
-        <f t="shared" ref="M11" si="6">65535/(I11-H11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N11" s="7">
-        <f t="shared" ref="N11" si="7">1/M11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O11" s="7">
-        <f t="shared" ref="O11" si="8">1/M11</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P11" s="12">
-        <f t="shared" ref="P11" si="9">ROUND((F11-H11)*M11,0)</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>6000</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -1554,219 +1530,219 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="16">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>65535</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" ref="M12" si="6">65535/(I12-H12)</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="7">
+        <f t="shared" ref="N12" si="7">1/M12</f>
+        <v>1</v>
+      </c>
+      <c r="O12" s="7">
+        <f t="shared" ref="O12" si="8">1/M12</f>
+        <v>1</v>
+      </c>
+      <c r="P12" s="12">
+        <f t="shared" ref="P12" si="9">ROUND((F12-H12)*M12,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="16">
         <v>0.1</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F13" s="16">
         <f t="shared" si="5"/>
         <v>22000</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G13" s="16">
         <v>22000</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H13" s="16">
         <v>15000</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I13" s="16">
         <v>30000</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="M12" s="7">
+      <c r="J13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M13" s="7">
         <f t="shared" si="0"/>
         <v>4.3689999999999998</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N13" s="7">
         <f t="shared" si="1"/>
         <v>0.22888532845044635</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O13" s="7">
         <f t="shared" si="2"/>
         <v>0.22888532845044635</v>
       </c>
-      <c r="P12" s="12">
+      <c r="P13" s="12">
         <f t="shared" si="3"/>
         <v>30583</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="16">
+      <c r="C14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="16">
         <v>0.1</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F14" s="16">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G14" s="16">
         <v>2000</v>
       </c>
-      <c r="H13" s="16">
-        <v>0</v>
-      </c>
-      <c r="I13" s="16">
+      <c r="H14" s="16">
+        <v>0</v>
+      </c>
+      <c r="I14" s="16">
         <v>20000</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="M13" s="7">
+      <c r="J14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M14" s="7">
         <f t="shared" si="0"/>
         <v>3.2767499999999998</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N14" s="7">
         <f t="shared" si="1"/>
         <v>0.30518043793392846</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O14" s="7">
         <f t="shared" si="2"/>
         <v>0.30518043793392846</v>
       </c>
-      <c r="P13" s="12">
+      <c r="P14" s="12">
         <f t="shared" si="3"/>
         <v>6554</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="16">
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
         <v>0.1</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F15" s="16">
         <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G15" s="16">
         <v>2.5</v>
       </c>
-      <c r="H14" s="16">
-        <v>0</v>
-      </c>
-      <c r="I14" s="16">
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="I15" s="16">
         <v>100</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="M14" s="7">
+      <c r="J15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M15" s="7">
         <f t="shared" si="0"/>
         <v>655.35</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N15" s="7">
         <f t="shared" si="1"/>
         <v>1.5259021896696422E-3</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O15" s="7">
         <f t="shared" si="2"/>
         <v>1.5259021896696422E-3</v>
       </c>
-      <c r="P14" s="12">
+      <c r="P15" s="12">
         <f t="shared" si="3"/>
         <v>1638</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>10</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" si="5"/>
-        <v>600</v>
-      </c>
-      <c r="G15" s="2">
-        <v>600</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
-        <v>6553</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M15" s="7">
-        <f t="shared" ref="M15" si="10">65535/(I15-H15)</f>
-        <v>10.000763009308713</v>
-      </c>
-      <c r="N15" s="7">
-        <f t="shared" ref="N15" si="11">1/M15</f>
-        <v>9.9992370489051657E-2</v>
-      </c>
-      <c r="O15" s="7">
-        <f t="shared" ref="O15" si="12">1/M15</f>
-        <v>9.9992370489051657E-2</v>
-      </c>
-      <c r="P15" s="12">
-        <f t="shared" ref="P15" si="13">ROUND((F15-H15)*M15,0)</f>
-        <v>6000</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -1775,54 +1751,54 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="F16" s="3">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0</v>
-      </c>
-      <c r="I16" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>35</v>
+        <v>6000</v>
+      </c>
+      <c r="G16" s="2">
+        <v>6000</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>65535</v>
+      </c>
+      <c r="J16" s="2">
+        <v>10</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>46</v>
+        <v>131</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="M16" s="7">
-        <f t="shared" si="0"/>
-        <v>65.534999999999997</v>
+        <f t="shared" ref="M16" si="10">65535/(I16-H16)</f>
+        <v>1</v>
       </c>
       <c r="N16" s="7">
-        <f t="shared" si="1"/>
-        <v>1.5259021896696423E-2</v>
+        <f t="shared" ref="N16" si="11">1/M16</f>
+        <v>1</v>
       </c>
       <c r="O16" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5259021896696423E-2</v>
+        <f t="shared" ref="O16" si="12">1/M16</f>
+        <v>1</v>
       </c>
       <c r="P16" s="12">
-        <f t="shared" si="3"/>
-        <v>66</v>
+        <f t="shared" ref="P16" si="13">ROUND((F16-H16)*M16,0)</f>
+        <v>6000</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -1834,35 +1810,35 @@
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="1">
         <v>0.01</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>-500</v>
-      </c>
-      <c r="I17" s="3">
-        <v>500</v>
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1000</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M17" s="7">
         <f t="shared" si="0"/>
@@ -1878,7 +1854,7 @@
       </c>
       <c r="P17" s="12">
         <f t="shared" si="3"/>
-        <v>32768</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -1890,35 +1866,35 @@
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="1">
         <v>0.01</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
-        <v>1000</v>
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>-500</v>
+      </c>
+      <c r="I18" s="4">
+        <v>500</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M18" s="7">
         <f t="shared" si="0"/>
@@ -1934,7 +1910,7 @@
       </c>
       <c r="P18" s="12">
         <f t="shared" si="3"/>
-        <v>66</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -1946,35 +1922,35 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="1">
         <v>0.01</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>-500</v>
-      </c>
-      <c r="I19" s="3">
-        <v>500</v>
+        <v>1</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1000</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M19" s="7">
         <f t="shared" si="0"/>
@@ -1990,7 +1966,7 @@
       </c>
       <c r="P19" s="12">
         <f t="shared" si="3"/>
-        <v>32768</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -2002,35 +1978,35 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D20" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1">
         <v>0.01</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="G20" s="3">
-        <v>1</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>1000</v>
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>-500</v>
+      </c>
+      <c r="I20" s="4">
+        <v>500</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>37</v>
+        <v>137</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M20" s="7">
         <f t="shared" si="0"/>
@@ -2046,7 +2022,7 @@
       </c>
       <c r="P20" s="12">
         <f t="shared" si="3"/>
-        <v>66</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -2055,332 +2031,52 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21" s="1">
         <v>0.01</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
-        <v>-500</v>
-      </c>
-      <c r="I21" s="3">
-        <v>500</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>37</v>
+        <v>1</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>10</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="M21" s="7">
         <f t="shared" si="0"/>
-        <v>65.534999999999997</v>
+        <v>6553.5</v>
       </c>
       <c r="N21" s="7">
         <f t="shared" si="1"/>
-        <v>1.5259021896696423E-2</v>
+        <v>1.5259021896696422E-4</v>
       </c>
       <c r="O21" s="7">
         <f t="shared" si="2"/>
-        <v>1.5259021896696423E-2</v>
+        <v>1.5259021896696422E-4</v>
       </c>
       <c r="P21" s="12">
-        <f t="shared" si="3"/>
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="F22" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="G22" s="3">
-        <v>1</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0</v>
-      </c>
-      <c r="I22" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M22" s="7">
-        <f t="shared" si="0"/>
-        <v>65.534999999999997</v>
-      </c>
-      <c r="N22" s="7">
-        <f t="shared" si="1"/>
-        <v>1.5259021896696423E-2</v>
-      </c>
-      <c r="O22" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5259021896696423E-2</v>
-      </c>
-      <c r="P22" s="12">
-        <f t="shared" si="3"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="1">
-        <v>2</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="3">
-        <v>0</v>
-      </c>
-      <c r="H23" s="3">
-        <v>-500</v>
-      </c>
-      <c r="I23" s="3">
-        <v>500</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M23" s="7">
-        <f t="shared" si="0"/>
-        <v>65.534999999999997</v>
-      </c>
-      <c r="N23" s="7">
-        <f t="shared" si="1"/>
-        <v>1.5259021896696423E-2</v>
-      </c>
-      <c r="O23" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5259021896696423E-2</v>
-      </c>
-      <c r="P23" s="12">
-        <f t="shared" si="3"/>
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <f t="shared" si="4"/>
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="F24" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="G24" s="3">
-        <v>1</v>
-      </c>
-      <c r="H24" s="3">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3">
-        <v>1000</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" s="7">
-        <f t="shared" si="0"/>
-        <v>65.534999999999997</v>
-      </c>
-      <c r="N24" s="7">
-        <f t="shared" si="1"/>
-        <v>1.5259021896696423E-2</v>
-      </c>
-      <c r="O24" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5259021896696423E-2</v>
-      </c>
-      <c r="P24" s="12">
-        <f t="shared" si="3"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <f t="shared" si="4"/>
-        <v>23</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="1">
-        <v>2</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="F25" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
-        <v>-500</v>
-      </c>
-      <c r="I25" s="3">
-        <v>500</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M25" s="7">
-        <f t="shared" si="0"/>
-        <v>65.534999999999997</v>
-      </c>
-      <c r="N25" s="7">
-        <f t="shared" si="1"/>
-        <v>1.5259021896696423E-2</v>
-      </c>
-      <c r="O25" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5259021896696423E-2</v>
-      </c>
-      <c r="P25" s="12">
-        <f t="shared" si="3"/>
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="1">
-        <v>3</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="F26" s="4">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="G26" s="4">
-        <v>1</v>
-      </c>
-      <c r="H26" s="4">
-        <v>0</v>
-      </c>
-      <c r="I26" s="4">
-        <v>10</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M26" s="7">
-        <f t="shared" si="0"/>
-        <v>6553.5</v>
-      </c>
-      <c r="N26" s="7">
-        <f t="shared" si="1"/>
-        <v>1.5259021896696422E-4</v>
-      </c>
-      <c r="O26" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5259021896696422E-4</v>
-      </c>
-      <c r="P26" s="12">
         <f t="shared" si="3"/>
         <v>6554</v>
       </c>
@@ -2395,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931DECF4-8BF0-4C1D-87E4-E5713582A1AF}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,7 +2114,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -2427,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -2439,7 +2135,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -2448,28 +2144,28 @@
         <v>1</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f>MAX(params_data!A:A)+1</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -2484,13 +2180,13 @@
         <v>65535</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="K2" s="7">
         <f t="shared" ref="K2:K25" si="0">65535/(G2-F2)</f>
@@ -2512,13 +2208,13 @@
     <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -2533,13 +2229,13 @@
         <v>65535</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" si="0"/>
@@ -2561,13 +2257,13 @@
     <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A25" si="4">A3+1</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -2582,13 +2278,13 @@
         <v>600</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="0"/>
@@ -2610,13 +2306,13 @@
     <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
@@ -2631,13 +2327,13 @@
         <v>50</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="0"/>
@@ -2659,13 +2355,13 @@
     <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="4"/>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
@@ -2680,13 +2376,13 @@
         <v>600</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="K6" s="7">
         <f t="shared" si="0"/>
@@ -2708,13 +2404,13 @@
     <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
@@ -2729,13 +2425,13 @@
         <v>50</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="0"/>
@@ -2757,13 +2453,13 @@
     <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="4"/>
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
@@ -2778,13 +2474,13 @@
         <v>180</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="0"/>
@@ -2806,13 +2502,13 @@
     <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
@@ -2827,13 +2523,13 @@
         <v>180</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="0"/>
@@ -2855,13 +2551,13 @@
     <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
@@ -2876,13 +2572,13 @@
         <v>100</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="0"/>
@@ -2904,13 +2600,13 @@
     <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -2925,13 +2621,13 @@
         <v>50000</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="0"/>
@@ -2953,13 +2649,13 @@
     <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="4"/>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -2971,28 +2667,28 @@
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>6553</v>
+        <v>65535</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" ref="K12" si="5">65535/(G12-F12)</f>
-        <v>10.000763009308713</v>
+        <v>1</v>
       </c>
       <c r="L12" s="7">
         <f t="shared" ref="L12" si="6">1/K12</f>
-        <v>9.9992370489051657E-2</v>
+        <v>1</v>
       </c>
       <c r="M12" s="7">
         <f t="shared" ref="M12" si="7">1/K12</f>
-        <v>9.9992370489051657E-2</v>
+        <v>1</v>
       </c>
       <c r="N12" s="15">
         <f t="shared" ref="N12" si="8">ROUND((E12-F12)*K12,0)</f>
@@ -3002,13 +2698,13 @@
     <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -3020,28 +2716,28 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>6553</v>
+        <v>65535</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="0"/>
-        <v>10.000763009308713</v>
+        <v>1</v>
       </c>
       <c r="L13" s="7">
         <f t="shared" si="2"/>
-        <v>9.9992370489051657E-2</v>
+        <v>1</v>
       </c>
       <c r="M13" s="7">
         <f t="shared" si="1"/>
-        <v>9.9992370489051657E-2</v>
+        <v>1</v>
       </c>
       <c r="N13" s="15">
         <f t="shared" si="3"/>
@@ -3051,13 +2747,13 @@
     <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="4"/>
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -3072,13 +2768,13 @@
         <v>65535</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="0"/>
@@ -3100,13 +2796,13 @@
     <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -3121,13 +2817,13 @@
         <v>65535</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="K15" s="7">
         <f t="shared" si="0"/>
@@ -3149,13 +2845,13 @@
     <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="4"/>
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -3170,13 +2866,13 @@
         <v>65535</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="0"/>
@@ -3198,13 +2894,13 @@
     <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -3219,13 +2915,13 @@
         <v>65535</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="K17" s="7">
         <f t="shared" si="0"/>
@@ -3247,13 +2943,13 @@
     <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -3268,13 +2964,13 @@
         <v>65535</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="K18" s="7">
         <f t="shared" si="0"/>
@@ -3296,13 +2992,13 @@
     <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -3317,13 +3013,13 @@
         <v>65535</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="0"/>
@@ -3345,13 +3041,13 @@
     <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="4"/>
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -3366,13 +3062,13 @@
         <v>65535</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="K20" s="7">
         <f t="shared" si="0"/>
@@ -3394,13 +3090,13 @@
     <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -3415,13 +3111,13 @@
         <v>65535</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="K21" s="7">
         <f t="shared" si="0"/>
@@ -3443,13 +3139,13 @@
     <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="4"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -3464,13 +3160,13 @@
         <v>65535</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="K22" s="7">
         <f t="shared" si="0"/>
@@ -3492,13 +3188,13 @@
     <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -3513,13 +3209,13 @@
         <v>65535</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" ref="K23" si="9">65535/(G23-F23)</f>
@@ -3541,13 +3237,13 @@
     <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
@@ -3562,13 +3258,13 @@
         <v>1</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="K24" s="7">
         <f>65535/(G24-F24)</f>
@@ -3590,13 +3286,13 @@
     <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
@@ -3611,13 +3307,13 @@
         <v>65</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="0"/>
@@ -3647,15 +3343,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9A672A-3BE0-43E6-9150-51A939FD7C9B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3687,26 +3383,26 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>

</xml_diff>